<commit_message>
second day, added most fuctionality, only graph
</commit_message>
<xml_diff>
--- a/patients/GeorgeGrgis.xlsx
+++ b/patients/GeorgeGrgis.xlsx
@@ -1,94 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Desktop\Stuffs\Projects\Programming\Current\Patient Diagram Maker\patient-diagram-maker\patients\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1406A7-D8FB-46A7-9598-E99613BC4187}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="2625" yWindow="1785" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
-  <si>
-    <t>Temp</t>
-  </si>
-  <si>
-    <t>Medication</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>30/12/2019</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>30/12/2020</t>
-  </si>
-  <si>
-    <t>30/12/2021</t>
-  </si>
-  <si>
-    <t>30/12/2022</t>
-  </si>
-  <si>
-    <t>30/12/2023</t>
-  </si>
-  <si>
-    <t>30/12/2024</t>
-  </si>
-  <si>
-    <t>30/12/2025</t>
-  </si>
-  <si>
-    <t>30/12/2026</t>
-  </si>
-  <si>
-    <t>amoxicillin-25mg;</t>
-  </si>
-  <si>
-    <t>amoxicillin-25mg;cefalexin-25mg;</t>
-  </si>
-  <si>
-    <t>amoxicillin-25mg;cefalexin-25mg;fajskllkds-26mg;</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -103,18 +46,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -122,24 +57,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -427,150 +353,334 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="38.42578125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Temp</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Meds</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>36.0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>30/12/2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>37.0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>30/12/2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>38.0</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>30/12/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>39.0</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>30/12/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>37</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>40.0</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>amoxicillin-25mg;</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>30/12/2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>41.0</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>amoxicillin-25mg;cefalexin-25mg;fajskllkds-26mg;</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>30/12/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>39</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>39.0</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>amoxicillin-25mg;cefalexin-25mg;</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>40</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>36.6</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>amoxicillin-25mg;cefalexin-25mg;fajskllkds-26mg;</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>30/12/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>39.0</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>amoxicillin-25mg;</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>30/12/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>amoxicillin-25mg;</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>31/12/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>amoxicillin-25mg;</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>01/01/2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>amoxicillin-25mg;</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>02/01/2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>41</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>amoxicillin-25mg;</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>03/01/2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>amoxicillin-25mg;</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>04/01/2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>39</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>36.6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>amoxicillin-25mg;</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>05/01/2023</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>